<commit_message>
📚 docs: The project documentation was updated along with the images of the results obtained.
</commit_message>
<xml_diff>
--- a/example_db/example.xlsx
+++ b/example_db/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2023105\Documents\Documentos\Proyectos\Generador_tablas\example_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AE7A82-1301-4E7D-AB2F-D4F2C1110E6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E931364-3BEC-47DF-8BCD-3A473071D8EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>DISAGGREGATE</t>
   </si>
   <si>
-    <t>${multiply},Expansion_factor</t>
+    <t>P2 - Test question 2,${multiply},Expansion_factor</t>
   </si>
 </sst>
 </file>
@@ -495,11 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -759,7 +758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -782,7 +781,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -805,7 +804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -828,7 +827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -851,7 +850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -871,7 +870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -894,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -917,7 +916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -940,7 +939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -963,7 +962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -987,18 +986,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G21" xr:uid="{0A6C1E0C-0C02-4642-8FB5-A729994EABCD}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="TEST1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G21" xr:uid="{0A6C1E0C-0C02-4642-8FB5-A729994EABCD}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1008,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70059C02-607F-4E26-B8F7-BF41B7AF98E1}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,8 +1037,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>

</xml_diff>